<commit_message>
Updated Large_Caps.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Large_Caps.xlsx
+++ b/NAV/Large_Caps.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J615"/>
+  <dimension ref="A1:J636"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A583" workbookViewId="0">
       <selection activeCell="G589" sqref="G589"/>
@@ -19274,6 +19274,657 @@
         <v>218.9484263325294</v>
       </c>
     </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2024-08-28</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>1713.5</v>
+      </c>
+      <c r="D616" t="n">
+        <v>611.2000122070312</v>
+      </c>
+      <c r="E616" t="n">
+        <v>1138.300048828125</v>
+      </c>
+      <c r="F616" t="n">
+        <v>180.9600067138672</v>
+      </c>
+      <c r="G616" t="n">
+        <v>641.5499877929688</v>
+      </c>
+      <c r="H616" t="n">
+        <v>22112.82034301758</v>
+      </c>
+      <c r="I616" t="n">
+        <v>0</v>
+      </c>
+      <c r="J616" t="n">
+        <v>218.9484263325294</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="C617" t="n">
+        <v>1755.650024414062</v>
+      </c>
+      <c r="D617" t="n">
+        <v>603.6199951171875</v>
+      </c>
+      <c r="E617" t="n">
+        <v>1132.050048828125</v>
+      </c>
+      <c r="F617" t="n">
+        <v>179.9400024414062</v>
+      </c>
+      <c r="G617" t="n">
+        <v>644.2999877929688</v>
+      </c>
+      <c r="H617" t="n">
+        <v>22256.81030273438</v>
+      </c>
+      <c r="I617" t="n">
+        <v>0.006511605371146772</v>
+      </c>
+      <c r="J617" t="n">
+        <v>220.3741320814404</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C618" t="n">
+        <v>1783.050048828125</v>
+      </c>
+      <c r="D618" t="n">
+        <v>600.3599853515625</v>
+      </c>
+      <c r="E618" t="n">
+        <v>1127.900024414062</v>
+      </c>
+      <c r="F618" t="n">
+        <v>178.6199951171875</v>
+      </c>
+      <c r="G618" t="n">
+        <v>632.0499877929688</v>
+      </c>
+      <c r="H618" t="n">
+        <v>22286.13012695312</v>
+      </c>
+      <c r="I618" t="n">
+        <v>0.001317341695415713</v>
+      </c>
+      <c r="J618" t="n">
+        <v>220.6644401142224</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C619" t="n">
+        <v>1840.550048828125</v>
+      </c>
+      <c r="D619" t="n">
+        <v>608.5800170898438</v>
+      </c>
+      <c r="E619" t="n">
+        <v>1111.550048828125</v>
+      </c>
+      <c r="F619" t="n">
+        <v>177.5399932861328</v>
+      </c>
+      <c r="G619" t="n">
+        <v>670.2000122070312</v>
+      </c>
+      <c r="H619" t="n">
+        <v>22669.95040893555</v>
+      </c>
+      <c r="I619" t="n">
+        <v>0.01722238359894636</v>
+      </c>
+      <c r="J619" t="n">
+        <v>224.4648077485163</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C620" t="n">
+        <v>1865.599975585938</v>
+      </c>
+      <c r="D620" t="n">
+        <v>599.9400024414062</v>
+      </c>
+      <c r="E620" t="n">
+        <v>1114</v>
+      </c>
+      <c r="F620" t="n">
+        <v>178.4600067138672</v>
+      </c>
+      <c r="G620" t="n">
+        <v>659.0999755859375</v>
+      </c>
+      <c r="H620" t="n">
+        <v>22746.27993774414</v>
+      </c>
+      <c r="I620" t="n">
+        <v>0.003366991432787071</v>
+      </c>
+      <c r="J620" t="n">
+        <v>225.2205788331677</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C621" t="n">
+        <v>1871.900024414062</v>
+      </c>
+      <c r="D621" t="n">
+        <v>609</v>
+      </c>
+      <c r="E621" t="n">
+        <v>1127.900024414062</v>
+      </c>
+      <c r="F621" t="n">
+        <v>176.0200042724609</v>
+      </c>
+      <c r="G621" t="n">
+        <v>650.8499755859375</v>
+      </c>
+      <c r="H621" t="n">
+        <v>22782.94021606445</v>
+      </c>
+      <c r="I621" t="n">
+        <v>0.001611704349926693</v>
+      </c>
+      <c r="J621" t="n">
+        <v>225.5835678197662</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C622" t="n">
+        <v>1864.949951171875</v>
+      </c>
+      <c r="D622" t="n">
+        <v>602.1799926757812</v>
+      </c>
+      <c r="E622" t="n">
+        <v>1115.150024414062</v>
+      </c>
+      <c r="F622" t="n">
+        <v>173.4799957275391</v>
+      </c>
+      <c r="G622" t="n">
+        <v>643.8499755859375</v>
+      </c>
+      <c r="H622" t="n">
+        <v>22586.02963256836</v>
+      </c>
+      <c r="I622" t="n">
+        <v>-0.008642896027846764</v>
+      </c>
+      <c r="J622" t="n">
+        <v>223.6338724975092</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C623" t="n">
+        <v>1857.150024414062</v>
+      </c>
+      <c r="D623" t="n">
+        <v>597.2999877929688</v>
+      </c>
+      <c r="E623" t="n">
+        <v>1100</v>
+      </c>
+      <c r="F623" t="n">
+        <v>169.8500061035156</v>
+      </c>
+      <c r="G623" t="n">
+        <v>634.7000122070312</v>
+      </c>
+      <c r="H623" t="n">
+        <v>22350.45025634766</v>
+      </c>
+      <c r="I623" t="n">
+        <v>-0.01043031378480992</v>
+      </c>
+      <c r="J623" t="n">
+        <v>221.301301034448</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C624" t="n">
+        <v>1860.449951171875</v>
+      </c>
+      <c r="D624" t="n">
+        <v>610.3400268554688</v>
+      </c>
+      <c r="E624" t="n">
+        <v>1104.150024414062</v>
+      </c>
+      <c r="F624" t="n">
+        <v>168.3300018310547</v>
+      </c>
+      <c r="G624" t="n">
+        <v>635.2000122070312</v>
+      </c>
+      <c r="H624" t="n">
+        <v>22404.27005004883</v>
+      </c>
+      <c r="I624" t="n">
+        <v>0.002407995950143633</v>
+      </c>
+      <c r="J624" t="n">
+        <v>221.8341936711005</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C625" t="n">
+        <v>1824.5</v>
+      </c>
+      <c r="D625" t="n">
+        <v>608</v>
+      </c>
+      <c r="E625" t="n">
+        <v>1113.199951171875</v>
+      </c>
+      <c r="F625" t="n">
+        <v>169.75</v>
+      </c>
+      <c r="G625" t="n">
+        <v>637.0499877929688</v>
+      </c>
+      <c r="H625" t="n">
+        <v>22289.99975585938</v>
+      </c>
+      <c r="I625" t="n">
+        <v>-0.005100380147810443</v>
+      </c>
+      <c r="J625" t="n">
+        <v>220.7027549535948</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C626" t="n">
+        <v>1833.150024414062</v>
+      </c>
+      <c r="D626" t="n">
+        <v>627.6599731445312</v>
+      </c>
+      <c r="E626" t="n">
+        <v>1112.599975585938</v>
+      </c>
+      <c r="F626" t="n">
+        <v>165.8800048828125</v>
+      </c>
+      <c r="G626" t="n">
+        <v>627.2000122070312</v>
+      </c>
+      <c r="H626" t="n">
+        <v>22284.95007324219</v>
+      </c>
+      <c r="I626" t="n">
+        <v>-0.0002265447587481507</v>
+      </c>
+      <c r="J626" t="n">
+        <v>220.6527559012188</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C627" t="n">
+        <v>1854.849975585938</v>
+      </c>
+      <c r="D627" t="n">
+        <v>645.5999755859375</v>
+      </c>
+      <c r="E627" t="n">
+        <v>1120.099975585938</v>
+      </c>
+      <c r="F627" t="n">
+        <v>167.0200042724609</v>
+      </c>
+      <c r="G627" t="n">
+        <v>651.0999755859375</v>
+      </c>
+      <c r="H627" t="n">
+        <v>22615.88967895508</v>
+      </c>
+      <c r="I627" t="n">
+        <v>0.01485036334500268</v>
+      </c>
+      <c r="J627" t="n">
+        <v>223.9295294994281</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C628" t="n">
+        <v>1894.449951171875</v>
+      </c>
+      <c r="D628" t="n">
+        <v>646.6500244140625</v>
+      </c>
+      <c r="E628" t="n">
+        <v>1118.550048828125</v>
+      </c>
+      <c r="F628" t="n">
+        <v>167.25</v>
+      </c>
+      <c r="G628" t="n">
+        <v>633.4500122070312</v>
+      </c>
+      <c r="H628" t="n">
+        <v>22746.35009765625</v>
+      </c>
+      <c r="I628" t="n">
+        <v>0.005768529142701387</v>
+      </c>
+      <c r="J628" t="n">
+        <v>225.221273516257</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C629" t="n">
+        <v>1857.599975585938</v>
+      </c>
+      <c r="D629" t="n">
+        <v>621.0499877929688</v>
+      </c>
+      <c r="E629" t="n">
+        <v>1115.849975585938</v>
+      </c>
+      <c r="F629" t="n">
+        <v>163.9600067138672</v>
+      </c>
+      <c r="G629" t="n">
+        <v>665.9500122070312</v>
+      </c>
+      <c r="H629" t="n">
+        <v>22506.51992797852</v>
+      </c>
+      <c r="I629" t="n">
+        <v>-0.01054367705799297</v>
+      </c>
+      <c r="J629" t="n">
+        <v>222.8466131417117</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C630" t="n">
+        <v>1848.699951171875</v>
+      </c>
+      <c r="D630" t="n">
+        <v>649.6500244140625</v>
+      </c>
+      <c r="E630" t="n">
+        <v>1110.949951171875</v>
+      </c>
+      <c r="F630" t="n">
+        <v>160.6000061035156</v>
+      </c>
+      <c r="G630" t="n">
+        <v>666.3499755859375</v>
+      </c>
+      <c r="H630" t="n">
+        <v>22484.49969482422</v>
+      </c>
+      <c r="I630" t="n">
+        <v>-0.0009783935155129372</v>
+      </c>
+      <c r="J630" t="n">
+        <v>222.6285814604598</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>1888.199951171875</v>
+      </c>
+      <c r="D631" t="n">
+        <v>646.7000122070312</v>
+      </c>
+      <c r="E631" t="n">
+        <v>1079.949951171875</v>
+      </c>
+      <c r="F631" t="n">
+        <v>158.5599975585938</v>
+      </c>
+      <c r="G631" t="n">
+        <v>651.7000122070312</v>
+      </c>
+      <c r="H631" t="n">
+        <v>22442.71960449219</v>
+      </c>
+      <c r="I631" t="n">
+        <v>-0.00185817300358472</v>
+      </c>
+      <c r="J631" t="n">
+        <v>222.2148990405636</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C632" t="n">
+        <v>1890.400024414062</v>
+      </c>
+      <c r="D632" t="n">
+        <v>652.1500244140625</v>
+      </c>
+      <c r="E632" t="n">
+        <v>1054.449951171875</v>
+      </c>
+      <c r="F632" t="n">
+        <v>155.25</v>
+      </c>
+      <c r="G632" t="n">
+        <v>649.5999755859375</v>
+      </c>
+      <c r="H632" t="n">
+        <v>22292.29992675781</v>
+      </c>
+      <c r="I632" t="n">
+        <v>-0.006702381903139165</v>
+      </c>
+      <c r="J632" t="n">
+        <v>220.7255299226262</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C633" t="n">
+        <v>1916.800048828125</v>
+      </c>
+      <c r="D633" t="n">
+        <v>654.4500122070312</v>
+      </c>
+      <c r="E633" t="n">
+        <v>1054.599975585938</v>
+      </c>
+      <c r="F633" t="n">
+        <v>161.4299926757812</v>
+      </c>
+      <c r="G633" t="n">
+        <v>665.1500244140625</v>
+      </c>
+      <c r="H633" t="n">
+        <v>22632.26013183594</v>
+      </c>
+      <c r="I633" t="n">
+        <v>0.01525011803156592</v>
+      </c>
+      <c r="J633" t="n">
+        <v>224.0916203065262</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C634" t="n">
+        <v>1919.949951171875</v>
+      </c>
+      <c r="D634" t="n">
+        <v>654.0999755859375</v>
+      </c>
+      <c r="E634" t="n">
+        <v>1055.25</v>
+      </c>
+      <c r="F634" t="n">
+        <v>159.5599975585938</v>
+      </c>
+      <c r="G634" t="n">
+        <v>672</v>
+      </c>
+      <c r="H634" t="n">
+        <v>22635.46960449219</v>
+      </c>
+      <c r="I634" t="n">
+        <v>0.0001418096397599883</v>
+      </c>
+      <c r="J634" t="n">
+        <v>224.1233986584751</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="C635" t="n">
+        <v>1904.650024414062</v>
+      </c>
+      <c r="D635" t="n">
+        <v>646.8499755859375</v>
+      </c>
+      <c r="E635" t="n">
+        <v>1051.550048828125</v>
+      </c>
+      <c r="F635" t="n">
+        <v>158.7400054931641</v>
+      </c>
+      <c r="G635" t="n">
+        <v>675.25</v>
+      </c>
+      <c r="H635" t="n">
+        <v>22510.13034057617</v>
+      </c>
+      <c r="I635" t="n">
+        <v>-0.005537294613544976</v>
+      </c>
+      <c r="J635" t="n">
+        <v>222.8823613703141</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="C636" t="n">
+        <v>1928.5</v>
+      </c>
+      <c r="D636" t="n">
+        <v>633.2999877929688</v>
+      </c>
+      <c r="E636" t="n">
+        <v>1063.449951171875</v>
+      </c>
+      <c r="F636" t="n">
+        <v>156.9400024414062</v>
+      </c>
+      <c r="G636" t="n">
+        <v>667.3499755859375</v>
+      </c>
+      <c r="H636" t="n">
+        <v>22551.57971191406</v>
+      </c>
+      <c r="I636" t="n">
+        <v>0.001841365230265907</v>
+      </c>
+      <c r="J636" t="n">
+        <v>223.292769200981</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>